<commit_message>
Accessory edit and update
</commit_message>
<xml_diff>
--- a/public/phu-lieu.xlsx
+++ b/public/phu-lieu.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>NGÀY</t>
   </si>
@@ -81,9 +81,6 @@
   </si>
   <si>
     <t>color</t>
-  </si>
-  <si>
-    <t>cuộn</t>
   </si>
   <si>
     <t>met</t>
@@ -454,7 +451,7 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -495,7 +492,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J1" s="9" t="s">
         <v>8</v>
@@ -509,7 +506,7 @@
         <v>45555</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C2" s="6">
         <v>8666</v>
@@ -530,7 +527,7 @@
         <v>14</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J2">
         <v>100</v>
@@ -541,7 +538,7 @@
         <v>45556</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" s="6">
         <v>1340</v>
@@ -559,10 +556,10 @@
         <v>12</v>
       </c>
       <c r="H3" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="I3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J3">
         <v>200</v>
@@ -573,7 +570,7 @@
         <v>45557</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" s="6">
         <v>4544</v>
@@ -591,10 +588,10 @@
         <v>11</v>
       </c>
       <c r="H4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J4">
         <v>100</v>

</xml_diff>